<commit_message>
- Modifications for ELECON_D (VARS etc)
</commit_message>
<xml_diff>
--- a/TempSensIDs.xlsx
+++ b/TempSensIDs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="196">
   <si>
     <t>ID</t>
   </si>
@@ -600,6 +600,12 @@
   </si>
   <si>
     <t>43</t>
+  </si>
+  <si>
+    <t>T_ELECON_D</t>
+  </si>
+  <si>
+    <t>1C</t>
   </si>
 </sst>
 </file>
@@ -674,9 +680,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="cs-CZ"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -701,7 +705,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="0.22657303794276121"/>
-                  <c:y val="-0.11516209387666156"/>
+                  <c:y val="-0.11516209387666158"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -989,11 +993,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="48163840"/>
-        <c:axId val="48038656"/>
+        <c:axId val="167388288"/>
+        <c:axId val="167389824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48163840"/>
+        <c:axId val="167388288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1002,12 +1006,12 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48038656"/>
+        <c:crossAx val="167389824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48038656"/>
+        <c:axId val="167389824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1016,14 +1020,13 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48163840"/>
+        <c:crossAx val="167388288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1061,7 +1064,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="0.30301713170389988"/>
-                  <c:y val="-1.1566724530270487E-3"/>
+                  <c:y val="-1.1566724530270491E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1153,11 +1156,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="48088576"/>
-        <c:axId val="48090112"/>
+        <c:axId val="167595392"/>
+        <c:axId val="167621760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48088576"/>
+        <c:axId val="167595392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1166,12 +1169,12 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48090112"/>
+        <c:crossAx val="167621760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48090112"/>
+        <c:axId val="167621760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1180,14 +1183,13 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48088576"/>
+        <c:crossAx val="167595392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1209,9 +1211,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="3.4883422180923114E-2"/>
-          <c:y val="3.237987078538266E-2"/>
-          <c:w val="0.62415285045891111"/>
+          <c:x val="3.4883422180923135E-2"/>
+          <c:y val="3.2379870785382681E-2"/>
+          <c:w val="0.62415285045891133"/>
           <c:h val="0.8841212396527357"/>
         </c:manualLayout>
       </c:layout>
@@ -1237,7 +1239,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.36746199941822061"/>
+                  <c:x val="0.36746199941822072"/>
                   <c:y val="-0.52618488794669849"/>
                 </c:manualLayout>
               </c:layout>
@@ -1377,8 +1379,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.48195106976662166"/>
-                  <c:y val="-0.37042070462346144"/>
+                  <c:x val="0.48195106976662178"/>
+                  <c:y val="-0.37042070462346166"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1434,11 +1436,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="48490368"/>
-        <c:axId val="48491904"/>
+        <c:axId val="168845312"/>
+        <c:axId val="168846848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48490368"/>
+        <c:axId val="168845312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4.0000000000000022E-2"/>
@@ -1448,12 +1450,12 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48491904"/>
+        <c:crossAx val="168846848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48491904"/>
+        <c:axId val="168846848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1462,7 +1464,7 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48490368"/>
+        <c:crossAx val="168845312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1474,7 +1476,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.69878260869565212"/>
-          <c:y val="0.21100696547546977"/>
+          <c:y val="0.21100696547546988"/>
           <c:w val="0.13323875733679741"/>
           <c:h val="0.28979027861901885"/>
         </c:manualLayout>
@@ -1880,10 +1882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:R42"/>
+  <dimension ref="A2:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:N42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3761,6 +3763,49 @@
       <c r="R42" t="str">
         <f>CONCATENATE("#define      ",A42,"            ",P42)</f>
         <v>#define      T_ELECON            39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
+      <c r="A43" t="s">
+        <v>194</v>
+      </c>
+      <c r="B43">
+        <v>41</v>
+      </c>
+      <c r="E43">
+        <v>28</v>
+      </c>
+      <c r="F43">
+        <v>52</v>
+      </c>
+      <c r="G43">
+        <v>99</v>
+      </c>
+      <c r="H43" t="s">
+        <v>166</v>
+      </c>
+      <c r="I43" t="s">
+        <v>167</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43" t="s">
+        <v>195</v>
+      </c>
+      <c r="N43" t="str">
+        <f t="shared" ref="N43" si="6">CONCATENATE("{0x",E43,",  0x",F43,",  0x",G43,",  0x",H43,",  0x",I43,",  0x",J43,", 0x",K43,",  0x",L43,"},                      //",A43)</f>
+        <v>{0x28,  0x52,  0x99,  0x7E,  0x0C,  0x0, 0x0,  0x1C},                      //T_ELECON_D</v>
+      </c>
+      <c r="P43">
+        <v>40</v>
+      </c>
+      <c r="R43" t="str">
+        <f>CONCATENATE("#define      ",A43,"            ",P43)</f>
+        <v>#define      T_ELECON_D            40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>